<commit_message>
Solved another DP Question successfully!
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/longest-common-subsequence/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock cooldown DP</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-with-cooldown/</t>
   </si>
 </sst>
 </file>
@@ -74,10 +80,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,7 +590,8 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="9.7734375"/>
-    <col bestFit="1" min="3" max="3" width="66.26171875"/>
+    <col bestFit="1" min="2" max="2" width="17.203125"/>
+    <col bestFit="1" min="3" max="3" width="70.18359375"/>
     <col bestFit="1" min="4" max="4" width="21.69140625"/>
   </cols>
   <sheetData>
@@ -612,9 +620,21 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="3">
+        <v>46093</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="C3"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Solved stock qn with txn fees using recursion + memoization
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-with-cooldown/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock with txn fee DP</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-with-transaction-fee/</t>
   </si>
 </sst>
 </file>
@@ -590,8 +596,8 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="9.7734375"/>
-    <col bestFit="1" min="2" max="2" width="17.203125"/>
-    <col bestFit="1" min="3" max="3" width="70.18359375"/>
+    <col bestFit="1" min="2" max="2" width="19.00390625"/>
+    <col bestFit="1" min="3" max="3" width="74.83203125"/>
     <col bestFit="1" min="4" max="4" width="21.69140625"/>
   </cols>
   <sheetData>
@@ -621,20 +627,32 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="3">
-        <v>46093</v>
+      <c r="A3" s="1">
+        <v>46065</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="3">
+        <v>46066</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
     <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="C4"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Solved Edit Distances DP using both Recursion + Memoization & Tabulation but got 4 methods to solve this question
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-with-transaction-fee/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Opns. to convert w1 to w2</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/edit-distance/</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="9.7734375"/>
-    <col bestFit="1" min="2" max="2" width="19.00390625"/>
+    <col bestFit="1" min="2" max="2" width="27.2421875"/>
     <col bestFit="1" min="3" max="3" width="74.83203125"/>
     <col bestFit="1" min="4" max="4" width="21.69140625"/>
   </cols>
@@ -638,7 +644,7 @@
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>46066</v>
       </c>
       <c r="B4" t="s">
@@ -646,6 +652,17 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="3">
+        <v>46067</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -653,6 +670,7 @@
     <hyperlink r:id="rId1" ref="C2"/>
     <hyperlink r:id="rId2" ref="C3"/>
     <hyperlink r:id="rId3" ref="C4"/>
+    <hyperlink r:id="rId4" ref="C5"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Solved DP Knapsack Problem using Recursion+Memoization and Tabulation Methods
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/edit-distance/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP Knapsack</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/0-1-knapsack-problem0945/1</t>
   </si>
 </sst>
 </file>
@@ -655,7 +661,7 @@
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>46067</v>
       </c>
       <c r="B5" t="s">
@@ -663,6 +669,17 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="3">
+        <v>46067</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -671,6 +688,7 @@
     <hyperlink r:id="rId2" ref="C3"/>
     <hyperlink r:id="rId3" ref="C4"/>
     <hyperlink r:id="rId4" ref="C5"/>
+    <hyperlink r:id="rId5" ref="C6"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Solved Counting Bits problem using brute-force iterative and with simple recursion and with recursion+memoization and with tabulation approaches
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/problems/0-1-knapsack-problem0945/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counting bits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/counting-bits/</t>
   </si>
 </sst>
 </file>
@@ -672,7 +678,7 @@
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>46067</v>
       </c>
       <c r="B6" t="s">
@@ -680,6 +686,17 @@
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="3">
+        <v>46068</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -689,6 +706,7 @@
     <hyperlink r:id="rId3" ref="C4"/>
     <hyperlink r:id="rId4" ref="C5"/>
     <hyperlink r:id="rId5" ref="C6"/>
+    <hyperlink r:id="rId6" ref="C7"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Solved another bit manipulation problem known as Single Number
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/counting-bits/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-number/</t>
   </si>
 </sst>
 </file>
@@ -689,7 +695,7 @@
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>46068</v>
       </c>
       <c r="B7" t="s">
@@ -697,6 +703,17 @@
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="3">
+        <v>46069</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -707,6 +724,7 @@
     <hyperlink r:id="rId4" ref="C5"/>
     <hyperlink r:id="rId5" ref="C6"/>
     <hyperlink r:id="rId6" ref="C7"/>
+    <hyperlink r:id="rId7" ref="C8"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Solved bit manipulation and Tries questions
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>date</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/single-number/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min flips to make a OR b = c</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-flips-to-make-a-or-b-equal-to-c/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Trie (Prefix Tree)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-trie-prefix-tree/</t>
   </si>
 </sst>
 </file>
@@ -706,7 +718,7 @@
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>46069</v>
       </c>
       <c r="B8" t="s">
@@ -714,6 +726,28 @@
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="3">
+        <v>46073</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="3">
+        <v>46074</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -725,6 +759,8 @@
     <hyperlink r:id="rId5" ref="C6"/>
     <hyperlink r:id="rId6" ref="C7"/>
     <hyperlink r:id="rId7" ref="C8"/>
+    <hyperlink r:id="rId8" ref="C9"/>
+    <hyperlink r:id="rId9" ref="C10"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Solved search suggestion problem using Linear, binary searches and also using Tries
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>date</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Suggestion System</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-suggestions-system/description/</t>
   </si>
 </sst>
 </file>
@@ -729,7 +735,7 @@
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <v>46073</v>
       </c>
       <c r="B9" t="s">
@@ -740,7 +746,7 @@
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>46074</v>
       </c>
       <c r="B10" t="s">
@@ -748,6 +754,17 @@
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="3">
+        <v>46075</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -761,6 +778,7 @@
     <hyperlink r:id="rId7" ref="C8"/>
     <hyperlink r:id="rId8" ref="C9"/>
     <hyperlink r:id="rId9" ref="C10"/>
+    <hyperlink r:id="rId10" ref="C11"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved non-overlapping qn using greedy
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>date</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/search-suggestions-system/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Overlapping Intervals</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/non-overlapping-intervals/</t>
   </si>
 </sst>
 </file>
@@ -757,7 +763,7 @@
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>46075</v>
       </c>
       <c r="B11" t="s">
@@ -765,6 +771,17 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="3">
+        <v>46076</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -779,6 +796,7 @@
     <hyperlink r:id="rId8" ref="C9"/>
     <hyperlink r:id="rId9" ref="C10"/>
     <hyperlink r:id="rId10" ref="C11"/>
+    <hyperlink r:id="rId11" ref="C12"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved daily temperatures qn. using monotonic stack
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>date</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/non-overlapping-intervals/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min. No. of arrows for bursting ballooons</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily Temperatures</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/daily-temperatures/</t>
   </si>
 </sst>
 </file>
@@ -644,8 +656,8 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="9.7734375"/>
-    <col bestFit="1" min="2" max="2" width="27.2421875"/>
-    <col bestFit="1" min="3" max="3" width="74.83203125"/>
+    <col bestFit="1" min="2" max="2" width="35.98046875"/>
+    <col bestFit="1" min="3" max="3" width="79.98046875"/>
     <col bestFit="1" min="4" max="4" width="21.69140625"/>
   </cols>
   <sheetData>
@@ -774,7 +786,7 @@
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="3">
+      <c r="A12" s="1">
         <v>46076</v>
       </c>
       <c r="B12" t="s">
@@ -782,6 +794,28 @@
       </c>
       <c r="C12" s="2" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="3">
+        <v>46077</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="3">
+        <v>46078</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -797,6 +831,8 @@
     <hyperlink r:id="rId9" ref="C10"/>
     <hyperlink r:id="rId10" ref="C11"/>
     <hyperlink r:id="rId11" ref="C12"/>
+    <hyperlink r:id="rId12" ref="C13"/>
+    <hyperlink r:id="rId13" ref="C14"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved online stock span qn. using monotonic stack
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>date</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/daily-temperatures/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online Stock Span</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/online-stock-span/</t>
   </si>
 </sst>
 </file>
@@ -797,7 +803,7 @@
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="3">
+      <c r="A13" s="1">
         <v>46077</v>
       </c>
       <c r="B13" t="s">
@@ -808,7 +814,7 @@
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="3">
+      <c r="A14" s="1">
         <v>46078</v>
       </c>
       <c r="B14" t="s">
@@ -816,6 +822,17 @@
       </c>
       <c r="C14" s="2" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="3">
+        <v>46079</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -833,6 +850,7 @@
     <hyperlink r:id="rId11" ref="C12"/>
     <hyperlink r:id="rId12" ref="C13"/>
     <hyperlink r:id="rId13" ref="C14"/>
+    <hyperlink r:id="rId14" ref="C15"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved merge 2 sorted arrays problem
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>date</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/online-stock-span/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leetcode 150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge 2 Sorted Arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-sorted-array/</t>
   </si>
 </sst>
 </file>
@@ -661,7 +670,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="9.7734375"/>
+    <col bestFit="1" min="1" max="1" width="12.30078125"/>
     <col bestFit="1" min="2" max="2" width="35.98046875"/>
     <col bestFit="1" min="3" max="3" width="79.98046875"/>
     <col bestFit="1" min="4" max="4" width="21.69140625"/>
@@ -825,7 +834,7 @@
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="3">
+      <c r="A15" s="1">
         <v>46079</v>
       </c>
       <c r="B15" t="s">
@@ -833,6 +842,22 @@
       </c>
       <c r="C15" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="3">
+        <v>46079</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -851,6 +876,7 @@
     <hyperlink r:id="rId12" ref="C13"/>
     <hyperlink r:id="rId13" ref="C14"/>
     <hyperlink r:id="rId14" ref="C15"/>
+    <hyperlink r:id="rId15" ref="C17"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved climb stairs and house robber DP Problems
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>date</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/merge-sorted-array/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climb Stairs</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House Robber</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/house-robber/description/</t>
   </si>
 </sst>
 </file>
@@ -850,7 +862,7 @@
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="3">
+      <c r="A17" s="1">
         <v>46079</v>
       </c>
       <c r="B17" t="s">
@@ -858,6 +870,28 @@
       </c>
       <c r="C17" s="2" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="1">
+        <v>46080</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="3">
+        <v>46080</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -877,6 +911,8 @@
     <hyperlink r:id="rId13" ref="C14"/>
     <hyperlink r:id="rId14" ref="C15"/>
     <hyperlink r:id="rId15" ref="C17"/>
+    <hyperlink r:id="rId16" ref="C18"/>
+    <hyperlink r:id="rId17" ref="C19"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved word break problem
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>date</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/house-robber/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word Break</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-break/description/</t>
   </si>
 </sst>
 </file>
@@ -884,7 +890,7 @@
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="3">
+      <c r="A19" s="1">
         <v>46080</v>
       </c>
       <c r="B19" t="s">
@@ -892,6 +898,17 @@
       </c>
       <c r="C19" s="2" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="3">
+        <v>46080</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -913,6 +930,7 @@
     <hyperlink r:id="rId15" ref="C17"/>
     <hyperlink r:id="rId16" ref="C18"/>
     <hyperlink r:id="rId17" ref="C19"/>
+    <hyperlink r:id="rId18" ref="C20"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved coin change problem
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>date</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/word-break/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coin Change</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/coin-change/description/</t>
   </si>
 </sst>
 </file>
@@ -901,7 +907,7 @@
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="3">
+      <c r="A20" s="1">
         <v>46080</v>
       </c>
       <c r="B20" t="s">
@@ -909,6 +915,17 @@
       </c>
       <c r="C20" s="2" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="3">
+        <v>46081</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -931,6 +948,7 @@
     <hyperlink r:id="rId16" ref="C18"/>
     <hyperlink r:id="rId17" ref="C19"/>
     <hyperlink r:id="rId18" ref="C20"/>
+    <hyperlink r:id="rId19" ref="C21"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved LIS problem using 3 approaches
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>date</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/coin-change/description/</t>
+  </si>
+  <si>
+    <t>LIS</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-increasing-subsequence/</t>
   </si>
 </sst>
 </file>
@@ -688,7 +694,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -918,7 +924,7 @@
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="3">
+      <c r="A21" s="1">
         <v>46081</v>
       </c>
       <c r="B21" t="s">
@@ -926,6 +932,17 @@
       </c>
       <c r="C21" s="2" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="3">
+        <v>46081</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -949,6 +966,7 @@
     <hyperlink r:id="rId17" ref="C19"/>
     <hyperlink r:id="rId18" ref="C20"/>
     <hyperlink r:id="rId19" ref="C21"/>
+    <hyperlink r:id="rId20" ref="C22"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
solved triangle problem using Multi-Dimensional DP
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>date</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/longest-increasing-subsequence/</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/triangle/</t>
   </si>
 </sst>
 </file>
@@ -195,7 +201,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,7 +700,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -935,7 +941,7 @@
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="3">
+      <c r="A22" s="1">
         <v>46081</v>
       </c>
       <c r="B22" t="s">
@@ -943,6 +949,17 @@
       </c>
       <c r="C22" s="2" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="3">
+        <v>46082</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -967,6 +984,7 @@
     <hyperlink r:id="rId18" ref="C20"/>
     <hyperlink r:id="rId19" ref="C21"/>
     <hyperlink r:id="rId20" ref="C22"/>
+    <hyperlink r:id="rId21" ref="C23"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
did min. path sum by myself
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>date</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/triangle/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min. Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-path-sum/</t>
   </si>
 </sst>
 </file>
@@ -201,7 +207,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,7 +706,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -953,13 +959,24 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="3">
-        <v>46082</v>
+        <v>46025</v>
       </c>
       <c r="B23" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="3">
+        <v>46025</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -985,6 +1002,7 @@
     <hyperlink r:id="rId19" ref="C21"/>
     <hyperlink r:id="rId20" ref="C22"/>
     <hyperlink r:id="rId21" ref="C23"/>
+    <hyperlink r:id="rId22" ref="C24"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
problem: unique paths II
</commit_message>
<xml_diff>
--- a/TrackingQuestions.xlsx
+++ b/TrackingQuestions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>date</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/minimum-path-sum/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Paths II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths-ii/</t>
   </si>
 </sst>
 </file>
@@ -958,7 +964,7 @@
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="3">
+      <c r="A23" s="1">
         <v>46025</v>
       </c>
       <c r="B23" t="s">
@@ -969,7 +975,7 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="3">
+      <c r="A24" s="1">
         <v>46025</v>
       </c>
       <c r="B24" t="s">
@@ -977,6 +983,17 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="3">
+        <v>46056</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1003,6 +1020,7 @@
     <hyperlink r:id="rId20" ref="C22"/>
     <hyperlink r:id="rId21" ref="C23"/>
     <hyperlink r:id="rId22" ref="C24"/>
+    <hyperlink r:id="rId23" ref="C25"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>